<commit_message>
add front end selecionar e emitir simples nacional
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACD7E9E-E167-49FC-BF84-FE36CEB82E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D834A6B3-B604-49C6-86ED-04C490CF7F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
   <si>
     <t>Telas</t>
   </si>
@@ -1435,7 +1435,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1554,7 +1554,9 @@
       <c r="C9" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1564,7 +1566,9 @@
       <c r="C10" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add front end importaçao de extrato
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D834A6B3-B604-49C6-86ED-04C490CF7F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB3CFC4-AE1D-4205-A4BB-D69FDC9FC965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="108">
   <si>
     <t>Telas</t>
   </si>
@@ -1435,7 +1435,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1578,7 +1578,9 @@
       <c r="C11" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add front end pagina de login (index)
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB3CFC4-AE1D-4205-A4BB-D69FDC9FC965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E7F791-812A-4FD3-9BE4-A88D438BF6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
   <si>
     <t>Telas</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Criar tela para gestão das página index</t>
   </si>
   <si>
-    <t>Criar tela de alteração de tela</t>
-  </si>
-  <si>
     <t>Consultar notas emitidas</t>
   </si>
   <si>
@@ -359,6 +356,15 @@
   </si>
   <si>
     <t>Criar tela editar de serviço</t>
+  </si>
+  <si>
+    <t>Criar tela de alteração de senha</t>
+  </si>
+  <si>
+    <t>Stand by</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -1413,16 +1419,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1432,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EE7D0D-B86C-4E32-A1E1-733236DDDE17}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,10 +1463,10 @@
         <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1471,7 +1477,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E2" s="12"/>
     </row>
@@ -1483,7 +1489,7 @@
         <v>0.125</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -1495,7 +1501,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" s="12"/>
     </row>
@@ -1507,43 +1513,43 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" s="12"/>
     </row>
@@ -1555,7 +1561,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E9" s="12"/>
     </row>
@@ -1567,7 +1573,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10" s="12"/>
     </row>
@@ -1579,18 +1585,20 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1605,7 +1613,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C14" s="1">
         <v>2.0833333333333332E-2</v>
@@ -1625,7 +1633,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1">
         <v>2.0833333333333332E-2</v>
@@ -1635,166 +1643,175 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="E18" s="12"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1">
-        <v>8.3333333333333329E-2</v>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1">
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
       <c r="C28" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="1">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
       <c r="C31" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C33" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="1">
-        <v>0.125</v>
+      <c r="C36" s="1">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C38" s="1">
         <v>0.125</v>
@@ -1802,7 +1819,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C39" s="1">
         <v>0.125</v>
@@ -1810,7 +1827,7 @@
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C40" s="1">
         <v>0.125</v>
@@ -1818,39 +1835,39 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C44" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1858,7 +1875,7 @@
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1866,39 +1883,39 @@
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" s="1">
-        <v>0.20833333333333334</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="1">
-        <v>0.125</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="1">
         <v>0.125</v>
@@ -1906,39 +1923,39 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C54" s="1">
-        <v>0.20833333333333334</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1946,7 +1963,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C57" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1954,7 +1971,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C58" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1962,9 +1979,17 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
         <v>80</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C60" s="1">
         <v>0.125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add front end consulta status nota fiscal
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E7F791-812A-4FD3-9BE4-A88D438BF6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86B43A0-37A7-484F-BDB1-D4E8CF481E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="110">
   <si>
     <t>Telas</t>
   </si>
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,7 +1638,9 @@
       <c r="C16" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add front end paginas perfil e recuperacao de senha
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86B43A0-37A7-484F-BDB1-D4E8CF481E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFF5467-48D0-4338-BDEC-AE17AFB05025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="111">
   <si>
     <t>Telas</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>está dentro da pagina perfil</t>
   </si>
 </sst>
 </file>
@@ -1438,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EE7D0D-B86C-4E32-A1E1-733236DDDE17}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1608,7 +1611,9 @@
       <c r="C13" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>103</v>
+      </c>
       <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1618,8 +1623,12 @@
       <c r="C14" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -1691,81 +1700,61 @@
         <v>103</v>
       </c>
     </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+      <c r="D21" s="12"/>
+    </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="12"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="12"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="12"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>28</v>
+      <c r="B28" t="s">
+        <v>35</v>
       </c>
       <c r="C28" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="1">
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>31</v>
+      <c r="B31" t="s">
+        <v>39</v>
       </c>
       <c r="C31" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1773,15 +1762,15 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>33</v>
+      <c r="B33" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C33" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1789,71 +1778,71 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C34" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C35" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>75</v>
+      <c r="B36" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C36" s="1">
         <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C38" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C39" s="1">
-        <v>0.125</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C40" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1">
         <v>0.125</v>
@@ -1861,31 +1850,31 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C44" s="1">
-        <v>0.5</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C46" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C47" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1893,23 +1882,23 @@
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C48" s="1">
-        <v>0.20833333333333334</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1">
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C50" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1917,31 +1906,31 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C53" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C54" s="1">
         <v>0.125</v>
@@ -1949,31 +1938,31 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C55" s="1">
-        <v>0.20833333333333334</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C56" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1981,17 +1970,57 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C59" s="1">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C65" s="1">
         <v>0.125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add front end paginas alertas, mensagens, tarefas e recuperação de senha
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFF5467-48D0-4338-BDEC-AE17AFB05025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983D150-215C-43FC-A6E4-F1FA24ACDCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
   <si>
     <t>Telas</t>
   </si>
@@ -368,6 +368,15 @@
   </si>
   <si>
     <t>está dentro da pagina perfil</t>
+  </si>
+  <si>
+    <t>Criar tela de alertas</t>
+  </si>
+  <si>
+    <t>Criar tela de mensagens</t>
+  </si>
+  <si>
+    <t>Criar tela de tarefas</t>
   </si>
 </sst>
 </file>
@@ -1443,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EE7D0D-B86C-4E32-A1E1-733236DDDE17}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1637,7 +1646,9 @@
       <c r="C15" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1701,16 +1712,37 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
-      <c r="D21" s="12"/>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="1"/>
-      <c r="D22" s="12"/>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-      <c r="D23" s="12"/>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>

</xml_diff>

<commit_message>
criado funcionalidade de consultar cnpj e cep atraves de api, criado modal para aviso para cadastro a atualização de cliente
</commit_message>
<xml_diff>
--- a/documentação/calculoOrçamentoContabilidade.xlsx
+++ b/documentação/calculoOrçamentoContabilidade.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983D150-215C-43FC-A6E4-F1FA24ACDCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D12539-3ABB-471E-B2B7-D18F40CB9AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{277B066D-FD2F-49A8-AD18-41178DF68479}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
   <si>
     <t>Telas</t>
   </si>
@@ -377,6 +377,12 @@
   </si>
   <si>
     <t>Criar tela de tarefas</t>
+  </si>
+  <si>
+    <t>Observação</t>
+  </si>
+  <si>
+    <t>Check</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EE7D0D-B86C-4E32-A1E1-733236DDDE17}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,12 +1468,12 @@
     <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1480,8 +1486,14 @@
       <c r="D1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -1493,7 +1505,7 @@
       </c>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>84</v>
       </c>
@@ -1505,7 +1517,7 @@
       </c>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>85</v>
       </c>
@@ -1517,7 +1529,7 @@
       </c>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>86</v>
       </c>
@@ -1529,7 +1541,7 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>104</v>
       </c>
@@ -1541,7 +1553,7 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>105</v>
       </c>
@@ -1553,7 +1565,7 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>106</v>
       </c>
@@ -1565,7 +1577,7 @@
       </c>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>87</v>
       </c>
@@ -1577,7 +1589,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>88</v>
       </c>
@@ -1589,7 +1601,7 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>89</v>
       </c>
@@ -1601,7 +1613,7 @@
       </c>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>101</v>
       </c>
@@ -1613,7 +1625,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>90</v>
       </c>
@@ -1625,7 +1637,7 @@
       </c>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>107</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>91</v>
       </c>
@@ -1651,7 +1663,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>92</v>
       </c>

</xml_diff>